<commit_message>
Format of figures and references im Text
</commit_message>
<xml_diff>
--- a/paper/supplementary_tables.xlsx
+++ b/paper/supplementary_tables.xlsx
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Hypo/anosmia</t>
+          <t>OD</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Hypo/ageusia</t>
+          <t>Hypogeusia/ageusia</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hypo/anosmia</t>
+          <t>OD</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2344,17 +2344,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>STDR</t>
+          <t>Cluster #1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>Cluster #2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>Cluster #3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -3122,17 +3122,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>STDR</t>
+          <t>Cluster #1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>Cluster #2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>Cluster #3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -3900,17 +3900,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>STDR</t>
+          <t>Cluster #1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>Cluster #2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>Cluster #3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -4392,17 +4392,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>STDR</t>
+          <t>Cluster #1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>Cluster #2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>Cluster #3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">

</xml_diff>